<commit_message>
Updates on run.R for py files Updates on time-series plots
</commit_message>
<xml_diff>
--- a/01_admin/outline.xlsx
+++ b/01_admin/outline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jumpeihirota/Desktop/Cloned因果推論/ClonedGZpj/01_admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB7631E-CD45-EA48-960B-9B0AFF6C00A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A493C6C6-365F-424E-9175-001A39889DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="500" windowWidth="24820" windowHeight="14900" xr2:uid="{8E56B4AF-C6FC-C449-B1FE-6FFCF4818F13}"/>
+    <workbookView xWindow="740" yWindow="500" windowWidth="24820" windowHeight="14900" xr2:uid="{8E56B4AF-C6FC-C449-B1FE-6FFCF4818F13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="33">
   <si>
     <t>Verb</t>
   </si>
@@ -124,16 +124,31 @@
   </si>
   <si>
     <t>Pop</t>
+  </si>
+  <si>
+    <t>Script</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>py</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -475,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9688FF-DFA8-FF40-8DA6-DD3C6C5A17E3}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,287 +502,404 @@
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
       <c r="B26" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>5</v>
       </c>
       <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
         <v>27</v>
       </c>
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code cleaning, folder restructuring, rmd file updates
</commit_message>
<xml_diff>
--- a/01_admin/outline.xlsx
+++ b/01_admin/outline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jumpeihirota/Desktop/Cloned因果推論/ClonedGZpj/01_admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E8293D-7027-2342-98B2-5C1A29AA36D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6378CBBC-F378-D045-BAD0-A88861E00A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="3040" windowWidth="24700" windowHeight="15500" xr2:uid="{8E56B4AF-C6FC-C449-B1FE-6FFCF4818F13}"/>
+    <workbookView xWindow="900" yWindow="500" windowWidth="24700" windowHeight="15500" xr2:uid="{8E56B4AF-C6FC-C449-B1FE-6FFCF4818F13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="30">
   <si>
     <t>Verb</t>
   </si>
@@ -72,18 +72,12 @@
     <t>Postas</t>
   </si>
   <si>
-    <t>Selfrestraint</t>
-  </si>
-  <si>
     <t>Dummy_vars</t>
   </si>
   <si>
     <t>GZ_covid</t>
   </si>
   <si>
-    <t>Pref_covid</t>
-  </si>
-  <si>
     <t>Controls</t>
   </si>
   <si>
@@ -102,47 +96,41 @@
     <t>Google Mobility</t>
   </si>
   <si>
-    <t>Res_view</t>
-  </si>
-  <si>
-    <t>Postas_plot</t>
-  </si>
-  <si>
-    <t>Postas_reg</t>
-  </si>
-  <si>
-    <t>Covid_reg_postas</t>
-  </si>
-  <si>
-    <t>Covid_reg_postas2</t>
+    <t>Google_mobility</t>
+  </si>
+  <si>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>Script</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>py</t>
+  </si>
+  <si>
+    <t>Robust_check</t>
+  </si>
+  <si>
+    <t>Stayhome_rate</t>
+  </si>
+  <si>
+    <t>Covid_reg</t>
   </si>
   <si>
     <t>Summary_stat</t>
   </si>
   <si>
-    <t>Google_mobility</t>
-  </si>
-  <si>
-    <t>Pop</t>
-  </si>
-  <si>
-    <t>Script</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>py</t>
-  </si>
-  <si>
-    <t>Robustness_check</t>
+    <t>GZlist_cum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,8 +144,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +162,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -183,9 +184,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9688FF-DFA8-FF40-8DA6-DD3C6C5A17E3}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -520,7 +524,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -531,7 +535,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -540,10 +544,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -552,10 +556,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -567,7 +571,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -579,7 +583,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -591,7 +595,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -603,7 +607,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -615,7 +619,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -627,7 +631,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -636,10 +640,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -648,10 +652,10 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -663,7 +667,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -672,10 +676,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -684,10 +688,10 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -696,115 +700,133 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
         <v>6</v>
       </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" t="s">
-        <v>33</v>
-      </c>
       <c r="C24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -812,118 +834,109 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" t="s">
-        <v>31</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D34" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Updates in plot files
</commit_message>
<xml_diff>
--- a/01_admin/outline.xlsx
+++ b/01_admin/outline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jumpeihirota/Desktop/Cloned因果推論/ClonedGZpj/01_admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50D4A35-01FE-FD43-99E2-D9C972EB4AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED18925D-6529-134E-8D9D-71C9C76F24F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="500" windowWidth="24700" windowHeight="15500" xr2:uid="{8E56B4AF-C6FC-C449-B1FE-6FFCF4818F13}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{8E56B4AF-C6FC-C449-B1FE-6FFCF4818F13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
   <si>
     <t>Verb</t>
   </si>
@@ -118,16 +118,13 @@
   </si>
   <si>
     <t>Covid</t>
-  </si>
-  <si>
-    <t>Gzlist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,15 +138,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,12 +149,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -181,11 +165,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -501,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9688FF-DFA8-FF40-8DA6-DD3C6C5A17E3}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -679,9 +661,9 @@
         <v>22</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -718,8 +700,8 @@
         <v>22</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -732,8 +714,8 @@
         <v>22</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -746,20 +728,20 @@
         <v>22</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -778,36 +760,36 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -819,7 +801,7 @@
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -828,12 +810,12 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -845,14 +827,14 @@
       <c r="C27" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
         <v>22</v>
@@ -864,24 +846,12 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
         <v>22</v>
       </c>
       <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>